<commit_message>
create modul update memebr
</commit_message>
<xml_diff>
--- a/ultah/ULTAH OKTOBER.xlsx
+++ b/ultah/ULTAH OKTOBER.xlsx
@@ -44,9 +44,6 @@
     <t>Riski Wahyudi</t>
   </si>
   <si>
-    <t>Bontokape, 01 Oktober 1997</t>
-  </si>
-  <si>
     <t>CW 5</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>I Komang Putra Pratangkas</t>
   </si>
   <si>
-    <t>Denpasar, 4 Oktober 1993</t>
-  </si>
-  <si>
     <t>CW 14</t>
   </si>
   <si>
@@ -119,13 +113,19 @@
     <t>TTL</t>
   </si>
   <si>
-    <t>DIVISI</t>
-  </si>
-  <si>
     <t>Banyuwangi, 15 Oktober 1994</t>
   </si>
   <si>
-    <t>Jember, 16 Oktober 1998</t>
+    <t>Denpasar, 04 Oktober 1993</t>
+  </si>
+  <si>
+    <t>Jember, 16-Oktober 1998</t>
+  </si>
+  <si>
+    <t>Bontokape, 01  - Oktober 1997</t>
+  </si>
+  <si>
+    <t>DEVISI</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,13 +150,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -197,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -212,12 +205,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -505,7 +492,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,15 +502,15 @@
     <col min="3" max="3" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -542,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -553,133 +540,134 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>